<commit_message>
Run the Notebook Scripts & Combine Scraping Results from Comments Presidential Debate Videos from the KPU RI YouTube Channel
</commit_message>
<xml_diff>
--- a/YouTube Channel KOMPASTV/Results of Data Exports from DataFrame/Export Comments Data from 3rd Video Debate.xlsx
+++ b/YouTube Channel KOMPASTV/Results of Data Exports from DataFrame/Export Comments Data from 3rd Video Debate.xlsx
@@ -7273,7 +7273,7 @@
         <v>1132</v>
       </c>
       <c r="F6">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -7561,7 +7561,7 @@
         <v>1141</v>
       </c>
       <c r="F15">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G15">
         <v>5</v>

</xml_diff>